<commit_message>
Old updates from local files
</commit_message>
<xml_diff>
--- a/utils/coc/analysisPackagesCoC - May-7-2025.xlsx
+++ b/utils/coc/analysisPackagesCoC - May-7-2025.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/jeremy_krogh_gov_bc_ca/Documents/Projects/2025/github_projects/aqs-api/utils/coc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/coc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{5EA246A0-82DC-4185-89D7-3105762A2B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3B3EC70-02C2-445A-95B7-5C229FC5F6E7}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{5EA246A0-82DC-4185-89D7-3105762A2B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A83F19EA-7EA5-4DF6-AE67-9D8989A27DC5}"/>
   <bookViews>
-    <workbookView xWindow="-14685" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$130</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -1017,21 +1020,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B102" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115:D125"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="5" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.54296875" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" customWidth="1"/>
+    <col min="4" max="5" width="43.26953125" customWidth="1"/>
     <col min="6" max="7" width="53" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>112</v>
       </c>
@@ -1080,7 +1083,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
@@ -1103,7 +1106,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>112</v>
       </c>
@@ -1126,7 +1129,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>112</v>
       </c>
@@ -1149,7 +1152,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>112</v>
       </c>
@@ -1172,7 +1175,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>112</v>
       </c>
@@ -1195,7 +1198,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>112</v>
       </c>
@@ -1218,7 +1221,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>112</v>
       </c>
@@ -1241,7 +1244,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>112</v>
       </c>
@@ -1264,7 +1267,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>112</v>
       </c>
@@ -1287,7 +1290,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>112</v>
       </c>
@@ -1310,7 +1313,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>112</v>
       </c>
@@ -1333,7 +1336,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>112</v>
       </c>
@@ -1356,7 +1359,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>112</v>
       </c>
@@ -1379,7 +1382,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>112</v>
       </c>
@@ -1402,7 +1405,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>112</v>
       </c>
@@ -1425,7 +1428,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>112</v>
       </c>
@@ -1448,7 +1451,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>112</v>
       </c>
@@ -1471,7 +1474,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>112</v>
       </c>
@@ -1494,7 +1497,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>112</v>
       </c>
@@ -1517,7 +1520,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>112</v>
       </c>
@@ -1540,7 +1543,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>112</v>
       </c>
@@ -1563,7 +1566,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>112</v>
       </c>
@@ -1586,7 +1589,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>112</v>
       </c>
@@ -1609,7 +1612,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>112</v>
       </c>
@@ -1632,7 +1635,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>112</v>
       </c>
@@ -1655,7 +1658,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>112</v>
       </c>
@@ -1678,7 +1681,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>112</v>
       </c>
@@ -1701,7 +1704,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>112</v>
       </c>
@@ -1724,7 +1727,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>112</v>
       </c>
@@ -1747,7 +1750,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>112</v>
       </c>
@@ -1770,7 +1773,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>112</v>
       </c>
@@ -1793,7 +1796,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>112</v>
       </c>
@@ -1816,7 +1819,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>112</v>
       </c>
@@ -1839,7 +1842,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>112</v>
       </c>
@@ -1862,7 +1865,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -1885,7 +1888,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -1908,7 +1911,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>112</v>
       </c>
@@ -1931,7 +1934,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>112</v>
       </c>
@@ -1954,7 +1957,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>112</v>
       </c>
@@ -1977,7 +1980,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>112</v>
       </c>
@@ -2000,7 +2003,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>112</v>
       </c>
@@ -2023,7 +2026,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>112</v>
       </c>
@@ -2046,7 +2049,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>112</v>
       </c>
@@ -2069,7 +2072,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>112</v>
       </c>
@@ -2092,7 +2095,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>112</v>
       </c>
@@ -2115,7 +2118,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>112</v>
       </c>
@@ -2138,7 +2141,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>112</v>
       </c>
@@ -2161,7 +2164,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>112</v>
       </c>
@@ -2184,7 +2187,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>112</v>
       </c>
@@ -2207,7 +2210,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>112</v>
       </c>
@@ -2230,7 +2233,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>112</v>
       </c>
@@ -2253,7 +2256,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>112</v>
       </c>
@@ -2276,7 +2279,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>112</v>
       </c>
@@ -2299,7 +2302,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>112</v>
       </c>
@@ -2322,7 +2325,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -2345,7 +2348,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>112</v>
       </c>
@@ -2368,7 +2371,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>112</v>
       </c>
@@ -2391,7 +2394,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>112</v>
       </c>
@@ -2414,7 +2417,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>112</v>
       </c>
@@ -2437,7 +2440,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>112</v>
       </c>
@@ -2462,7 +2465,7 @@
       </c>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>112</v>
       </c>
@@ -2487,7 +2490,7 @@
       </c>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>112</v>
       </c>
@@ -2512,7 +2515,7 @@
       </c>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>112</v>
       </c>
@@ -2535,7 +2538,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>112</v>
       </c>
@@ -2560,7 +2563,7 @@
       </c>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>112</v>
       </c>
@@ -2585,7 +2588,7 @@
       </c>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>112</v>
       </c>
@@ -2610,7 +2613,7 @@
       </c>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>112</v>
       </c>
@@ -2635,7 +2638,7 @@
       </c>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>112</v>
       </c>
@@ -2660,7 +2663,7 @@
       </c>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>112</v>
       </c>
@@ -2685,7 +2688,7 @@
       </c>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>112</v>
       </c>
@@ -2708,7 +2711,7 @@
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>112</v>
       </c>
@@ -2731,7 +2734,7 @@
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>112</v>
       </c>
@@ -2754,7 +2757,7 @@
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>112</v>
       </c>
@@ -2779,7 +2782,7 @@
       </c>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>112</v>
       </c>
@@ -2804,7 +2807,7 @@
       </c>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>112</v>
       </c>
@@ -2829,7 +2832,7 @@
       </c>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>112</v>
       </c>
@@ -2854,7 +2857,7 @@
       </c>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>112</v>
       </c>
@@ -2879,7 +2882,7 @@
       </c>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>112</v>
       </c>
@@ -2904,7 +2907,7 @@
       </c>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>112</v>
       </c>
@@ -2929,7 +2932,7 @@
       </c>
       <c r="I81" s="2"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>112</v>
       </c>
@@ -2954,7 +2957,7 @@
       </c>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>112</v>
       </c>
@@ -2979,7 +2982,7 @@
       </c>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>112</v>
       </c>
@@ -3004,7 +3007,7 @@
       </c>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>112</v>
       </c>
@@ -3029,7 +3032,7 @@
       </c>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>112</v>
       </c>
@@ -3054,7 +3057,7 @@
       </c>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>112</v>
       </c>
@@ -3079,7 +3082,7 @@
       </c>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>112</v>
       </c>
@@ -3104,7 +3107,7 @@
       </c>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>112</v>
       </c>
@@ -3129,7 +3132,7 @@
       </c>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>112</v>
       </c>
@@ -3144,7 +3147,7 @@
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>112</v>
       </c>
@@ -3169,7 +3172,7 @@
       </c>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>156</v>
       </c>
@@ -3192,7 +3195,7 @@
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>156</v>
       </c>
@@ -3215,7 +3218,7 @@
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>156</v>
       </c>
@@ -3238,7 +3241,7 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>156</v>
       </c>
@@ -3261,7 +3264,7 @@
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>156</v>
       </c>
@@ -3281,7 +3284,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>156</v>
       </c>
@@ -3304,7 +3307,7 @@
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>156</v>
       </c>
@@ -3327,7 +3330,7 @@
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>156</v>
       </c>
@@ -3350,7 +3353,7 @@
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>156</v>
       </c>
@@ -3373,7 +3376,7 @@
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
     </row>
-    <row r="101" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>156</v>
       </c>
@@ -3396,7 +3399,7 @@
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
     </row>
-    <row r="102" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>156</v>
       </c>
@@ -3419,7 +3422,7 @@
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
     </row>
-    <row r="103" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>156</v>
       </c>
@@ -3442,7 +3445,7 @@
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>156</v>
       </c>
@@ -3465,7 +3468,7 @@
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>156</v>
       </c>
@@ -3488,7 +3491,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>156</v>
       </c>
@@ -3508,7 +3511,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>156</v>
       </c>
@@ -3523,7 +3526,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>156</v>
       </c>
@@ -3543,7 +3546,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>155</v>
       </c>
@@ -3566,7 +3569,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>155</v>
       </c>
@@ -3589,7 +3592,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>155</v>
       </c>
@@ -3612,7 +3615,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>155</v>
       </c>
@@ -3635,7 +3638,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>155</v>
       </c>
@@ -3658,7 +3661,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>155</v>
       </c>
@@ -3681,7 +3684,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>155</v>
       </c>
@@ -3702,7 +3705,7 @@
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>190</v>
       </c>
@@ -3720,7 +3723,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>190</v>
       </c>
@@ -3738,7 +3741,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>190</v>
       </c>
@@ -3756,7 +3759,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>190</v>
       </c>
@@ -3774,7 +3777,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>190</v>
       </c>
@@ -3792,7 +3795,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>190</v>
       </c>
@@ -3810,7 +3813,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>190</v>
       </c>
@@ -3828,7 +3831,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>190</v>
       </c>
@@ -3846,7 +3849,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>190</v>
       </c>
@@ -3864,7 +3867,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>190</v>
       </c>
@@ -3882,7 +3885,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>190</v>
       </c>
@@ -3902,7 +3905,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>190</v>
       </c>
@@ -3922,7 +3925,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>190</v>
       </c>
@@ -3942,7 +3945,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>190</v>
       </c>
@@ -3962,7 +3965,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>190</v>
       </c>
@@ -3978,6 +3981,7 @@
       <c r="I130" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I130" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>